<commit_message>
Update to test plan file
</commit_message>
<xml_diff>
--- a/Frontier Landing Page Test Suite.xlsx
+++ b/Frontier Landing Page Test Suite.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="93">
   <si>
     <t>Dependencies:</t>
   </si>
@@ -295,6 +295,9 @@
   </si>
   <si>
     <t>Input fields are a likely place for potential issues</t>
+  </si>
+  <si>
+    <t>URL: https://internet.frontier.com/?lp=6108</t>
   </si>
 </sst>
 </file>
@@ -1087,7 +1090,7 @@
   <dimension ref="A1:H377"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+      <selection activeCell="B7" sqref="B7:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1177,7 +1180,9 @@
       <c r="A6" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="43"/>
+      <c r="B6" s="43" t="s">
+        <v>92</v>
+      </c>
       <c r="C6" s="44"/>
       <c r="D6" s="44"/>
       <c r="E6" s="44"/>

</xml_diff>